<commit_message>
#242 Support footer and header
PR #300
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls3/MultiSheetTest.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls3/MultiSheetTest.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\git-repos-2203\jxls3\jxls-poi\src\test\resources\org\jxls3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\2023Stuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1221EC-E822-4ACA-8C16-1D5689DC6353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA313EC-470C-4D46-AE00-99477D3B5958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CCFD295-1CCF-445D-9327-8EE5976927A7}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{6CCFD295-1CCF-445D-9327-8EE5976927A7}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">template!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -137,10 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -461,11 +463,11 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25"/>
@@ -473,7 +475,7 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -489,13 +491,16 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="1.1811023622047245" right="1.1811023622047245" top="1.1811023622047245" bottom="1.1811023622047245" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0">
+    <oddFooter>&amp;LA</oddFooter>
+  </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>